<commit_message>
Person 2 - Milestone 5: Tool Evaluation & Recommendation
- Added deployment tool comparison (CSV and Excel formats)
- Created Power BI integration script (powerbi_link.R)
- Generated Power BI data exports (CSV, JSON, Excel formats)
- Implemented tool evaluation with Power BI as primary choice
- All deliverables ready for Section 2 submission
</commit_message>
<xml_diff>
--- a/Milestone 5 outputs/Deployment_Exports/powerbi_data.xlsx
+++ b/Milestone 5 outputs/Deployment_Exports/powerbi_data.xlsx
@@ -6,15 +6,15 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="ModelMetrics" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="FeatureImportance" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Metadata" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Model Performance" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Feature Importance" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Deployment Info" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -73,43 +73,25 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
-    <t xml:space="preserve">Field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Export Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025-10-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Person 1 – Group M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milestone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milestone 5 – Deployment Phase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Models</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logistic Regression, Decision Tree, Random Forest, Naïve Bayes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R Version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Base Directory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C:/Users/modir/Downloads/HDPSA-BIN381-main (6)/HDPSA-BIN381-main</t>
+    <t xml:space="preserve">deployment_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refresh_frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDPSA Clean Dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekly</t>
   </si>
 </sst>
 </file>
@@ -117,13 +99,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,8 +133,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,55 +646,27 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>20</v>
+      <c r="A2" s="1" t="n">
+        <v>45944</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>